<commit_message>
Updated the product backlog to indicate the next item
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Current" sheetId="3" r:id="rId2"/>
-    <sheet name="Completed" sheetId="2" r:id="rId3"/>
+    <sheet name="Current" sheetId="3" r:id="rId1"/>
+    <sheet name="Completed" sheetId="2" r:id="rId2"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Description</t>
   </si>
@@ -36,15 +36,9 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Build framework for Java serverside components</t>
-  </si>
-  <si>
     <t>S000006</t>
   </si>
   <si>
-    <t>Implement cross-platform communication</t>
-  </si>
-  <si>
     <t>S000007</t>
   </si>
   <si>
@@ -58,6 +52,15 @@
   </si>
   <si>
     <t>User should be able to calculate bond coupon accrual by entering bond identifier and settlement date</t>
+  </si>
+  <si>
+    <t>Implement cross-platform communication using ProtoBuf</t>
+  </si>
+  <si>
+    <t>Build framework for Java serverside components using standard Java components and communication using RabbitMQ</t>
+  </si>
+  <si>
+    <t>Implement Java service to calculate bond coupon accrual using bond identifier and settlement date</t>
   </si>
 </sst>
 </file>
@@ -106,10 +109,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,9 +421,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="103" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -437,10 +516,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -451,89 +530,35 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>